<commit_message>
added wall thickness and pump sizing
</commit_message>
<xml_diff>
--- a/output_tables/pipe_pressure.xlsx
+++ b/output_tables/pipe_pressure.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-25695" yWindow="1050" windowWidth="23985" windowHeight="14535" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="384" yWindow="384" windowWidth="15036" windowHeight="14100" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="pressure_drop" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="wall_thickness" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="data" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="fittings" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="fittings" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -87,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -276,46 +275,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -336,6 +295,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thick">
         <color indexed="64"/>
       </top>
@@ -352,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -404,17 +392,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -436,9 +416,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -450,7 +427,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -602,94 +579,6 @@
         <a:xfrm>
           <a:off x="9436100" y="2026186"/>
           <a:ext cx="425450" cy="196361"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </twoCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <twoCellAnchor editAs="oneCell">
-    <from>
-      <col>2</col>
-      <colOff>355600</colOff>
-      <row>10</row>
-      <rowOff>101599</rowOff>
-    </from>
-    <to>
-      <col>3</col>
-      <colOff>495300</colOff>
-      <row>12</row>
-      <rowOff>44450</rowOff>
-    </to>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Picture 2"/>
-        <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </cNvPicPr>
-      </nvPicPr>
-      <blipFill rotWithShape="1">
-        <a:blip r:embed="rId1"/>
-        <a:srcRect t="17779" b="19992"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:xfrm>
-          <a:off x="1574800" y="2114549"/>
-          <a:ext cx="1530350" cy="311151"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </twoCellAnchor>
-  <twoCellAnchor editAs="oneCell">
-    <from>
-      <col>5</col>
-      <colOff>533400</colOff>
-      <row>10</row>
-      <rowOff>82551</rowOff>
-    </from>
-    <to>
-      <col>7</col>
-      <colOff>57150</colOff>
-      <row>12</row>
-      <rowOff>125267</rowOff>
-    </to>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Picture 3"/>
-        <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </cNvPicPr>
-      </nvPicPr>
-      <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:xfrm>
-          <a:off x="4743450" y="2095501"/>
-          <a:ext cx="1504950" cy="411016"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <avLst/>
@@ -1027,37 +916,37 @@
   </sheetPr>
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="21.77734375" customWidth="1" style="48" min="3" max="3"/>
-    <col width="15.21875" customWidth="1" style="48" min="4" max="4"/>
-    <col width="35.5546875" customWidth="1" style="48" min="5" max="5"/>
-    <col width="14.77734375" customWidth="1" style="48" min="6" max="6"/>
-    <col width="14.88671875" customWidth="1" style="48" min="7" max="7"/>
-    <col width="15.21875" customWidth="1" style="48" min="8" max="8"/>
+    <col width="21.77734375" customWidth="1" style="42" min="3" max="3"/>
+    <col width="15.21875" customWidth="1" style="42" min="4" max="4"/>
+    <col width="35.5546875" customWidth="1" style="42" min="5" max="5"/>
+    <col width="14.77734375" customWidth="1" style="42" min="6" max="6"/>
+    <col width="14.88671875" customWidth="1" style="42" min="7" max="7"/>
+    <col width="15.21875" customWidth="1" style="42" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.55" customHeight="1" s="48" thickBot="1">
-      <c r="A1" s="42" t="inlineStr">
+    <row r="1" ht="26.55" customHeight="1" s="42" thickBot="1">
+      <c r="A1" s="36" t="inlineStr">
         <is>
           <t>PIPING PRESSURE DROP CALCULATION</t>
         </is>
       </c>
-      <c r="B1" s="43" t="n"/>
-      <c r="C1" s="43" t="n"/>
-      <c r="D1" s="43" t="n"/>
-      <c r="E1" s="43" t="n"/>
-      <c r="F1" s="43" t="n"/>
-      <c r="G1" s="43" t="n"/>
-      <c r="H1" s="43" t="n"/>
-      <c r="I1" s="43" t="n"/>
-      <c r="J1" s="44" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="48" thickBot="1">
+      <c r="B1" s="37" t="n"/>
+      <c r="C1" s="37" t="n"/>
+      <c r="D1" s="37" t="n"/>
+      <c r="E1" s="37" t="n"/>
+      <c r="F1" s="37" t="n"/>
+      <c r="G1" s="37" t="n"/>
+      <c r="H1" s="37" t="n"/>
+      <c r="I1" s="37" t="n"/>
+      <c r="J1" s="38" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="42" thickBot="1">
       <c r="A2" s="15" t="n"/>
       <c r="B2" s="16" t="inlineStr">
         <is>
@@ -1080,10 +969,13 @@
           <t>Line Description:</t>
         </is>
       </c>
-      <c r="D3" s="57" t="n"/>
-      <c r="E3" s="58" t="n"/>
-      <c r="F3" s="58" t="n"/>
-      <c r="G3" s="58" t="n"/>
+      <c r="D3" s="50">
+        <f>data!B26</f>
+        <v/>
+      </c>
+      <c r="E3" s="51" t="n"/>
+      <c r="F3" s="51" t="n"/>
+      <c r="G3" s="51" t="n"/>
       <c r="J3" s="9" t="n"/>
     </row>
     <row r="4">
@@ -1097,8 +989,11 @@
           <t>Nominal Size</t>
         </is>
       </c>
-      <c r="D5" s="1" t="n"/>
-      <c r="F5" s="47" t="inlineStr">
+      <c r="D5" s="1">
+        <f>data!B27</f>
+        <v/>
+      </c>
+      <c r="F5" s="41" t="inlineStr">
         <is>
           <t>Absolute Roughness (ε)</t>
         </is>
@@ -1121,8 +1016,11 @@
           <t>Material and Schedule</t>
         </is>
       </c>
-      <c r="D6" s="46" t="n"/>
-      <c r="F6" s="47" t="inlineStr">
+      <c r="D6" s="40">
+        <f>data!B28</f>
+        <v/>
+      </c>
+      <c r="F6" s="41" t="inlineStr">
         <is>
           <t>Inside Diameter (d)</t>
         </is>
@@ -1138,43 +1036,43 @@
       </c>
       <c r="J6" s="9" t="n"/>
     </row>
-    <row r="7" ht="15" customHeight="1" s="48" thickBot="1">
+    <row r="7" ht="15" customHeight="1" s="42" thickBot="1">
       <c r="A7" s="12" t="n"/>
-      <c r="B7" s="52" t="n"/>
-      <c r="C7" s="52" t="n"/>
-      <c r="D7" s="52" t="n"/>
-      <c r="E7" s="52" t="n"/>
-      <c r="F7" s="51" t="inlineStr">
+      <c r="B7" s="46" t="n"/>
+      <c r="C7" s="46" t="n"/>
+      <c r="D7" s="46" t="n"/>
+      <c r="E7" s="46" t="n"/>
+      <c r="F7" s="45" t="inlineStr">
         <is>
           <t>Inside Diameter (D)</t>
         </is>
       </c>
-      <c r="G7" s="52" t="n"/>
-      <c r="H7" s="55">
+      <c r="G7" s="46" t="n"/>
+      <c r="H7" s="48">
         <f>data!B4</f>
         <v/>
       </c>
-      <c r="I7" s="52" t="inlineStr">
+      <c r="I7" s="46" t="inlineStr">
         <is>
           <t>m</t>
         </is>
       </c>
       <c r="J7" s="13" t="n"/>
     </row>
-    <row r="8" ht="15" customHeight="1" s="48" thickBot="1">
+    <row r="8" ht="15" customHeight="1" s="42" thickBot="1">
       <c r="A8" s="18" t="n"/>
-      <c r="B8" s="56" t="inlineStr">
+      <c r="B8" s="49" t="inlineStr">
         <is>
           <t>Fluid Properties</t>
         </is>
       </c>
-      <c r="C8" s="52" t="n"/>
-      <c r="D8" s="52" t="n"/>
-      <c r="E8" s="52" t="n"/>
-      <c r="F8" s="52" t="n"/>
-      <c r="G8" s="52" t="n"/>
-      <c r="H8" s="52" t="n"/>
-      <c r="I8" s="52" t="n"/>
+      <c r="C8" s="46" t="n"/>
+      <c r="D8" s="46" t="n"/>
+      <c r="E8" s="46" t="n"/>
+      <c r="F8" s="46" t="n"/>
+      <c r="G8" s="46" t="n"/>
+      <c r="H8" s="46" t="n"/>
+      <c r="I8" s="46" t="n"/>
       <c r="J8" s="19" t="n"/>
     </row>
     <row r="9">
@@ -1184,13 +1082,13 @@
           <t>Fluid:</t>
         </is>
       </c>
-      <c r="D9" s="58" t="n"/>
-      <c r="F9" s="47" t="inlineStr">
+      <c r="D9" s="51" t="n"/>
+      <c r="F9" s="41" t="inlineStr">
         <is>
           <t>Average Pressure:</t>
         </is>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="51">
         <f>data!B6</f>
         <v/>
       </c>
@@ -1208,7 +1106,7 @@
           <t>Flow Rate (W):</t>
         </is>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="40">
         <f>data!B5</f>
         <v/>
       </c>
@@ -1217,7 +1115,7 @@
           <t>kg / hr</t>
         </is>
       </c>
-      <c r="F10" s="47" t="inlineStr">
+      <c r="F10" s="41" t="inlineStr">
         <is>
           <t>Average Temperature:</t>
         </is>
@@ -1233,9 +1131,9 @@
       </c>
       <c r="J10" s="9" t="n"/>
     </row>
-    <row r="11" ht="16.5" customHeight="1" s="48">
+    <row r="11" ht="16.5" customHeight="1" s="42">
       <c r="A11" s="7" t="n"/>
-      <c r="F11" s="47" t="inlineStr">
+      <c r="F11" s="41" t="inlineStr">
         <is>
           <t>Specific Volume (V)</t>
         </is>
@@ -1247,7 +1145,7 @@
       <c r="J11" s="9" t="n"/>
     </row>
     <row r="12">
-      <c r="F12" s="47" t="inlineStr">
+      <c r="F12" s="41" t="inlineStr">
         <is>
           <t>Absolute Viscosity (μ)</t>
         </is>
@@ -1263,18 +1161,18 @@
       </c>
       <c r="J12" s="9" t="n"/>
     </row>
-    <row r="13" ht="15" customHeight="1" s="48" thickBot="1">
+    <row r="13" ht="15" customHeight="1" s="42" thickBot="1">
       <c r="A13" s="12" t="n"/>
-      <c r="B13" s="52" t="n"/>
-      <c r="C13" s="52" t="n"/>
-      <c r="D13" s="52" t="n"/>
-      <c r="E13" s="52" t="n"/>
-      <c r="F13" s="51" t="n"/>
-      <c r="G13" s="51" t="n"/>
-      <c r="I13" s="52" t="n"/>
+      <c r="B13" s="46" t="n"/>
+      <c r="C13" s="46" t="n"/>
+      <c r="D13" s="46" t="n"/>
+      <c r="E13" s="46" t="n"/>
+      <c r="F13" s="45" t="n"/>
+      <c r="G13" s="45" t="n"/>
+      <c r="I13" s="46" t="n"/>
       <c r="J13" s="13" t="n"/>
     </row>
-    <row r="14" ht="15" customHeight="1" s="48" thickBot="1">
+    <row r="14" ht="15" customHeight="1" s="42" thickBot="1">
       <c r="A14" s="15" t="n"/>
       <c r="B14" s="23" t="inlineStr">
         <is>
@@ -1290,7 +1188,7 @@
       <c r="I14" s="23" t="n"/>
       <c r="J14" s="17" t="n"/>
     </row>
-    <row r="15" ht="16.5" customHeight="1" s="48">
+    <row r="15" ht="16.5" customHeight="1" s="42">
       <c r="A15" s="7" t="n"/>
       <c r="C15" t="inlineStr">
         <is>
@@ -1322,7 +1220,7 @@
       </c>
       <c r="J15" s="9" t="n"/>
     </row>
-    <row r="16" ht="25.5" customHeight="1" s="48">
+    <row r="16" ht="25.5" customHeight="1" s="42">
       <c r="A16" s="7" t="n"/>
       <c r="C16" t="inlineStr">
         <is>
@@ -1344,7 +1242,7 @@
       </c>
       <c r="J16" s="9" t="n"/>
     </row>
-    <row r="17" ht="22.95" customHeight="1" s="48">
+    <row r="17" ht="22.95" customHeight="1" s="42">
       <c r="A17" s="7" t="n"/>
       <c r="C17" t="inlineStr">
         <is>
@@ -1353,7 +1251,7 @@
       </c>
       <c r="J17" s="9" t="n"/>
     </row>
-    <row r="18" ht="39.45" customHeight="1" s="48">
+    <row r="18" ht="39.45" customHeight="1" s="42">
       <c r="A18" s="7" t="n"/>
       <c r="C18" s="10" t="inlineStr">
         <is>
@@ -1366,7 +1264,7 @@
       </c>
       <c r="J18" s="9" t="n"/>
     </row>
-    <row r="19" ht="33.45" customHeight="1" s="48">
+    <row r="19" ht="33.45" customHeight="1" s="42">
       <c r="A19" s="7" t="n"/>
       <c r="C19" s="10" t="inlineStr">
         <is>
@@ -1380,7 +1278,7 @@
       </c>
       <c r="J19" s="9" t="n"/>
     </row>
-    <row r="20" ht="15" customHeight="1" s="48" thickBot="1">
+    <row r="20" ht="15" customHeight="1" s="42" thickBot="1">
       <c r="A20" s="7" t="n"/>
       <c r="C20" s="20" t="n"/>
       <c r="D20" s="20" t="n"/>
@@ -1391,7 +1289,7 @@
       <c r="I20" s="20" t="n"/>
       <c r="J20" s="9" t="n"/>
     </row>
-    <row r="21" ht="15.45" customHeight="1" s="48" thickBot="1" thickTop="1">
+    <row r="21" ht="15.45" customHeight="1" s="42" thickBot="1" thickTop="1">
       <c r="A21" s="7" t="n"/>
       <c r="C21" t="inlineStr">
         <is>
@@ -1415,24 +1313,24 @@
       </c>
       <c r="J21" s="9" t="n"/>
     </row>
-    <row r="22" ht="15" customHeight="1" s="48" thickTop="1">
+    <row r="22" ht="15" customHeight="1" s="42" thickTop="1">
       <c r="A22" s="7" t="n"/>
-      <c r="C22" s="49">
+      <c r="C22" s="43">
         <f>fittings!A2</f>
         <v/>
       </c>
-      <c r="D22" s="50" t="n"/>
-      <c r="E22" s="50" t="n"/>
-      <c r="F22" s="50" t="n"/>
-      <c r="G22" s="53">
+      <c r="D22" s="44" t="n"/>
+      <c r="E22" s="44" t="n"/>
+      <c r="F22" s="44" t="n"/>
+      <c r="G22" s="5">
         <f>fittings!B2</f>
         <v/>
       </c>
-      <c r="H22" s="53">
+      <c r="H22" s="5">
         <f>fittings!C2</f>
         <v/>
       </c>
-      <c r="I22" s="53">
+      <c r="I22" s="5">
         <f>fittings!D2</f>
         <v/>
       </c>
@@ -1440,22 +1338,22 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="n"/>
-      <c r="C23" s="45">
+      <c r="C23" s="39">
         <f>fittings!A3</f>
         <v/>
       </c>
-      <c r="D23" s="46" t="n"/>
-      <c r="E23" s="46" t="n"/>
-      <c r="F23" s="46" t="n"/>
-      <c r="G23" s="53">
+      <c r="D23" s="40" t="n"/>
+      <c r="E23" s="40" t="n"/>
+      <c r="F23" s="40" t="n"/>
+      <c r="G23" s="5">
         <f>fittings!B3</f>
         <v/>
       </c>
-      <c r="H23" s="53">
+      <c r="H23" s="5">
         <f>fittings!C3</f>
         <v/>
       </c>
-      <c r="I23" s="53">
+      <c r="I23" s="5">
         <f>fittings!D3</f>
         <v/>
       </c>
@@ -1463,22 +1361,22 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="n"/>
-      <c r="C24" s="45">
+      <c r="C24" s="39">
         <f>fittings!A4</f>
         <v/>
       </c>
-      <c r="D24" s="46" t="n"/>
-      <c r="E24" s="46" t="n"/>
-      <c r="F24" s="46" t="n"/>
-      <c r="G24" s="53">
+      <c r="D24" s="40" t="n"/>
+      <c r="E24" s="40" t="n"/>
+      <c r="F24" s="40" t="n"/>
+      <c r="G24" s="5">
         <f>fittings!B4</f>
         <v/>
       </c>
-      <c r="H24" s="53">
+      <c r="H24" s="5">
         <f>fittings!C4</f>
         <v/>
       </c>
-      <c r="I24" s="53">
+      <c r="I24" s="5">
         <f>fittings!D4</f>
         <v/>
       </c>
@@ -1486,22 +1384,22 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="n"/>
-      <c r="C25" s="45">
+      <c r="C25" s="39">
         <f>fittings!A5</f>
         <v/>
       </c>
-      <c r="D25" s="46" t="n"/>
-      <c r="E25" s="46" t="n"/>
-      <c r="F25" s="46" t="n"/>
-      <c r="G25" s="53">
+      <c r="D25" s="40" t="n"/>
+      <c r="E25" s="40" t="n"/>
+      <c r="F25" s="40" t="n"/>
+      <c r="G25" s="5">
         <f>fittings!B5</f>
         <v/>
       </c>
-      <c r="H25" s="53">
+      <c r="H25" s="5">
         <f>fittings!C5</f>
         <v/>
       </c>
-      <c r="I25" s="53">
+      <c r="I25" s="5">
         <f>fittings!D5</f>
         <v/>
       </c>
@@ -1509,22 +1407,22 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="n"/>
-      <c r="C26" s="45">
+      <c r="C26" s="39">
         <f>fittings!A6</f>
         <v/>
       </c>
-      <c r="D26" s="46" t="n"/>
-      <c r="E26" s="46" t="n"/>
-      <c r="F26" s="46" t="n"/>
-      <c r="G26" s="53">
+      <c r="D26" s="40" t="n"/>
+      <c r="E26" s="40" t="n"/>
+      <c r="F26" s="40" t="n"/>
+      <c r="G26" s="5">
         <f>fittings!B6</f>
         <v/>
       </c>
-      <c r="H26" s="53">
+      <c r="H26" s="5">
         <f>fittings!C6</f>
         <v/>
       </c>
-      <c r="I26" s="53">
+      <c r="I26" s="5">
         <f>fittings!D6</f>
         <v/>
       </c>
@@ -1532,22 +1430,22 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="n"/>
-      <c r="C27" s="45">
+      <c r="C27" s="39">
         <f>fittings!A7</f>
         <v/>
       </c>
-      <c r="D27" s="46" t="n"/>
-      <c r="E27" s="46" t="n"/>
-      <c r="F27" s="46" t="n"/>
-      <c r="G27" s="53">
+      <c r="D27" s="40" t="n"/>
+      <c r="E27" s="40" t="n"/>
+      <c r="F27" s="40" t="n"/>
+      <c r="G27" s="5">
         <f>fittings!B7</f>
         <v/>
       </c>
-      <c r="H27" s="53">
+      <c r="H27" s="5">
         <f>fittings!C7</f>
         <v/>
       </c>
-      <c r="I27" s="53">
+      <c r="I27" s="5">
         <f>fittings!D7</f>
         <v/>
       </c>
@@ -1555,22 +1453,22 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="n"/>
-      <c r="C28" s="45">
+      <c r="C28" s="39">
         <f>fittings!A8</f>
         <v/>
       </c>
-      <c r="D28" s="46" t="n"/>
-      <c r="E28" s="46" t="n"/>
-      <c r="F28" s="46" t="n"/>
-      <c r="G28" s="53">
+      <c r="D28" s="40" t="n"/>
+      <c r="E28" s="40" t="n"/>
+      <c r="F28" s="40" t="n"/>
+      <c r="G28" s="5">
         <f>fittings!B8</f>
         <v/>
       </c>
-      <c r="H28" s="53">
+      <c r="H28" s="5">
         <f>fittings!C8</f>
         <v/>
       </c>
-      <c r="I28" s="53">
+      <c r="I28" s="5">
         <f>fittings!D8</f>
         <v/>
       </c>
@@ -1578,36 +1476,36 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="n"/>
-      <c r="C29" s="45">
+      <c r="C29" s="39">
         <f>fittings!A9</f>
         <v/>
       </c>
-      <c r="D29" s="46" t="n"/>
-      <c r="E29" s="46" t="n"/>
-      <c r="F29" s="46" t="n"/>
-      <c r="G29" s="53">
+      <c r="D29" s="40" t="n"/>
+      <c r="E29" s="40" t="n"/>
+      <c r="F29" s="40" t="n"/>
+      <c r="G29" s="5">
         <f>fittings!B9</f>
         <v/>
       </c>
-      <c r="H29" s="53">
+      <c r="H29" s="5">
         <f>fittings!C9</f>
         <v/>
       </c>
-      <c r="I29" s="53">
+      <c r="I29" s="5">
         <f>fittings!D9</f>
         <v/>
       </c>
       <c r="J29" s="9" t="n"/>
     </row>
-    <row r="30" ht="15" customHeight="1" s="48" thickBot="1">
+    <row r="30" ht="15" customHeight="1" s="42" thickBot="1">
       <c r="A30" s="7" t="n"/>
-      <c r="C30" s="54">
+      <c r="C30" s="47">
         <f>fittings!A10</f>
         <v/>
       </c>
-      <c r="D30" s="55" t="n"/>
-      <c r="E30" s="55" t="n"/>
-      <c r="F30" s="55" t="n"/>
+      <c r="D30" s="48" t="n"/>
+      <c r="E30" s="48" t="n"/>
+      <c r="F30" s="48" t="n"/>
       <c r="G30" s="32">
         <f>fittings!B10</f>
         <v/>
@@ -1622,7 +1520,7 @@
       </c>
       <c r="J30" s="9" t="n"/>
     </row>
-    <row r="31" ht="15" customHeight="1" s="48">
+    <row r="31" ht="15" customHeight="1" s="42">
       <c r="A31" s="7" t="n"/>
       <c r="F31" s="6" t="inlineStr">
         <is>
@@ -1642,10 +1540,10 @@
       <c r="F32" s="6" t="n"/>
       <c r="G32" s="6" t="n"/>
       <c r="H32" s="6" t="n"/>
-      <c r="I32" s="53" t="n"/>
+      <c r="I32" s="5" t="n"/>
       <c r="J32" s="9" t="n"/>
     </row>
-    <row r="33" ht="16.5" customHeight="1" s="48">
+    <row r="33" ht="16.5" customHeight="1" s="42">
       <c r="A33" s="7" t="n"/>
       <c r="C33" t="inlineStr">
         <is>
@@ -1668,7 +1566,7 @@
       </c>
       <c r="J33" s="9" t="n"/>
     </row>
-    <row r="34" ht="16.5" customHeight="1" s="48">
+    <row r="34" ht="16.5" customHeight="1" s="42">
       <c r="A34" s="7" t="n"/>
       <c r="C34" t="inlineStr">
         <is>
@@ -1686,7 +1584,7 @@
       </c>
       <c r="J34" s="9" t="n"/>
     </row>
-    <row r="35" ht="16.5" customHeight="1" s="48">
+    <row r="35" ht="16.5" customHeight="1" s="42">
       <c r="A35" s="7" t="n"/>
       <c r="C35" t="inlineStr">
         <is>
@@ -1698,7 +1596,7 @@
           <t>L_TEL = L_F + L_P</t>
         </is>
       </c>
-      <c r="H35" s="46">
+      <c r="H35" s="40">
         <f>data!B18</f>
         <v/>
       </c>
@@ -1709,7 +1607,7 @@
       </c>
       <c r="J35" s="9" t="n"/>
     </row>
-    <row r="36" ht="17.55" customHeight="1" s="48">
+    <row r="36" ht="17.55" customHeight="1" s="42">
       <c r="A36" s="7" t="n"/>
       <c r="C36" t="inlineStr">
         <is>
@@ -1816,7 +1714,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="n"/>
-      <c r="F40" s="46" t="n"/>
+      <c r="F40" s="40" t="n"/>
       <c r="G40" t="inlineStr">
         <is>
           <t xml:space="preserve">m               = </t>
@@ -1834,7 +1732,7 @@
       <c r="A41" s="7" t="n"/>
       <c r="J41" s="9" t="n"/>
     </row>
-    <row r="42" ht="16.5" customHeight="1" s="48" thickBot="1">
+    <row r="42" ht="16.5" customHeight="1" s="42" thickBot="1">
       <c r="A42" s="7" t="n"/>
       <c r="C42" s="11" t="inlineStr">
         <is>
@@ -1852,16 +1750,16 @@
       </c>
       <c r="J42" s="9" t="n"/>
     </row>
-    <row r="43" ht="15.45" customHeight="1" s="48" thickBot="1" thickTop="1">
+    <row r="43" ht="15.45" customHeight="1" s="42" thickBot="1" thickTop="1">
       <c r="A43" s="12" t="n"/>
-      <c r="B43" s="52" t="n"/>
-      <c r="C43" s="52" t="n"/>
-      <c r="D43" s="52" t="n"/>
-      <c r="E43" s="52" t="n"/>
-      <c r="F43" s="52" t="n"/>
-      <c r="G43" s="52" t="n"/>
-      <c r="H43" s="52" t="n"/>
-      <c r="I43" s="52" t="n"/>
+      <c r="B43" s="46" t="n"/>
+      <c r="C43" s="46" t="n"/>
+      <c r="D43" s="46" t="n"/>
+      <c r="E43" s="46" t="n"/>
+      <c r="F43" s="46" t="n"/>
+      <c r="G43" s="46" t="n"/>
+      <c r="H43" s="46" t="n"/>
+      <c r="I43" s="46" t="n"/>
       <c r="J43" s="13" t="n"/>
     </row>
   </sheetData>
@@ -1893,414 +1791,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J26"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="19.88671875" customWidth="1" style="48" min="3" max="3"/>
-    <col width="14.21875" customWidth="1" style="48" min="4" max="4"/>
-    <col width="19.6640625" customWidth="1" style="48" min="6" max="6"/>
-    <col width="15.77734375" customWidth="1" style="48" min="8" max="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="26.55" customHeight="1" s="48" thickBot="1">
-      <c r="A1" s="42" t="inlineStr">
-        <is>
-          <t>MINIMUM WALL THICKNESS FOR PIPE UNDER INTERNAL PRESSURE</t>
-        </is>
-      </c>
-      <c r="B1" s="43" t="n"/>
-      <c r="C1" s="43" t="n"/>
-      <c r="D1" s="43" t="n"/>
-      <c r="E1" s="43" t="n"/>
-      <c r="F1" s="43" t="n"/>
-      <c r="G1" s="43" t="n"/>
-      <c r="H1" s="43" t="n"/>
-      <c r="I1" s="43" t="n"/>
-      <c r="J1" s="44" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="48" thickBot="1">
-      <c r="A2" s="15" t="n"/>
-      <c r="B2" s="16" t="inlineStr">
-        <is>
-          <t>Pipe and System Characteristics</t>
-        </is>
-      </c>
-      <c r="C2" s="16" t="n"/>
-      <c r="D2" s="16" t="n"/>
-      <c r="E2" s="16" t="n"/>
-      <c r="F2" s="16" t="n"/>
-      <c r="G2" s="16" t="n"/>
-      <c r="H2" s="16" t="n"/>
-      <c r="I2" s="16" t="n"/>
-      <c r="J2" s="17" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="n"/>
-      <c r="C3" s="8" t="n"/>
-      <c r="D3" s="53" t="n"/>
-      <c r="J3" s="9" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="n"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Pipeline Identification</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="n"/>
-      <c r="J4" s="9" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="n"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Applicable Pipe Sizes</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="n"/>
-      <c r="F5" s="47" t="inlineStr">
-        <is>
-          <t>Fluid</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="n"/>
-      <c r="J5" s="9" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="n"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>BREI Pipe Classification</t>
-        </is>
-      </c>
-      <c r="D6" s="46" t="n"/>
-      <c r="F6" s="47" t="inlineStr">
-        <is>
-          <t>Design Pressure (P)</t>
-        </is>
-      </c>
-      <c r="H6">
-        <f>data!B26</f>
-        <v/>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>bar (g)</t>
-        </is>
-      </c>
-      <c r="J6" s="9" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="n"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ASTM Specification</t>
-        </is>
-      </c>
-      <c r="D7" s="46" t="n"/>
-      <c r="F7" s="47" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Design Temperature </t>
-        </is>
-      </c>
-      <c r="H7" s="46">
-        <f>data!B27</f>
-        <v/>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J7" s="9" t="n"/>
-    </row>
-    <row r="8">
-      <c r="F8" s="47" t="n"/>
-      <c r="J8" s="9" t="n"/>
-    </row>
-    <row r="9" ht="15" customHeight="1" s="48" thickBot="1">
-      <c r="J9" s="13" t="n"/>
-    </row>
-    <row r="10" ht="15" customHeight="1" s="48" thickBot="1">
-      <c r="A10" s="15" t="n"/>
-      <c r="B10" s="16" t="inlineStr">
-        <is>
-          <t>Formula for Minimum Wall Thickness</t>
-        </is>
-      </c>
-      <c r="C10" s="16" t="n"/>
-      <c r="D10" s="16" t="n"/>
-      <c r="E10" s="16" t="n"/>
-      <c r="F10" s="16" t="n"/>
-      <c r="G10" s="16" t="n"/>
-      <c r="H10" s="16" t="n"/>
-      <c r="I10" s="16" t="n"/>
-      <c r="J10" s="17" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="37" t="n"/>
-      <c r="B11" s="38" t="n"/>
-      <c r="C11" s="38" t="n"/>
-      <c r="D11" s="38" t="n"/>
-      <c r="E11" s="38" t="n"/>
-      <c r="F11" s="38" t="n"/>
-      <c r="G11" s="38" t="n"/>
-      <c r="H11" s="38" t="n"/>
-      <c r="I11" s="38" t="n"/>
-      <c r="J11" s="39" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="n"/>
-      <c r="J12" s="9" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="n"/>
-      <c r="J13" s="9" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="n"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">P = </t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Internal Design Pressure</t>
-        </is>
-      </c>
-      <c r="J14" s="9" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="7" t="n"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">d = </t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Internal Diameter (mm)</t>
-        </is>
-      </c>
-      <c r="J15" s="9" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="7" t="n"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SE = </t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Maximum Allowable Stress Specified in B31.1 Appendix A = </t>
-        </is>
-      </c>
-      <c r="H16">
-        <f>data!B28</f>
-        <v/>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>bar</t>
-        </is>
-      </c>
-      <c r="J16" s="9" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="n"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Y = </t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Coefficient with Value Specified in B31.1 Table 104.1.2A = </t>
-        </is>
-      </c>
-      <c r="H17" s="36">
-        <f>data!B29</f>
-        <v/>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>mm</t>
-        </is>
-      </c>
-      <c r="J17" s="9" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="7" t="n"/>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A = </t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Additional Thickness Allowed for Corrosion, Erosion, and/or Mechanical Strength = </t>
-        </is>
-      </c>
-      <c r="H18" s="36">
-        <f>data!B30</f>
-        <v/>
-      </c>
-      <c r="J18" s="9" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="n"/>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MFG = </t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Manufacturer's Wall Thickness Tolerance = </t>
-        </is>
-      </c>
-      <c r="H19">
-        <f>data!B31</f>
-        <v/>
-      </c>
-      <c r="J19" s="9" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="7" t="n"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BEND = </t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Multiplier for Additional Thickness for Bending Specified in B31.1 Table  102.4.5</t>
-        </is>
-      </c>
-      <c r="H20">
-        <f>data!B32</f>
-        <v/>
-      </c>
-      <c r="J20" s="9" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="7" t="n"/>
-      <c r="J21" s="9" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="7" t="n"/>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">T_n  = </t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Nominal Wall Thickness Required (mm)</t>
-        </is>
-      </c>
-      <c r="H22" s="41">
-        <f>data!B33</f>
-        <v/>
-      </c>
-      <c r="I22" s="8" t="inlineStr">
-        <is>
-          <t>mm</t>
-        </is>
-      </c>
-      <c r="J22" s="9" t="n"/>
-    </row>
-    <row r="23" ht="15" customHeight="1" s="48">
-      <c r="B23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">T_m = </t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Minimum Wall Thickness (mm)</t>
-        </is>
-      </c>
-      <c r="H23" s="1">
-        <f>data!B34</f>
-        <v/>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>mm</t>
-        </is>
-      </c>
-      <c r="J23" s="9" t="n"/>
-    </row>
-    <row r="24" ht="15" customHeight="1" s="48">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">OD = </t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Outer Diameter (mm)</t>
-        </is>
-      </c>
-      <c r="H24" s="1">
-        <f>data!B35</f>
-        <v/>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>mm</t>
-        </is>
-      </c>
-      <c r="J24" s="9" t="n"/>
-    </row>
-    <row r="25" ht="15" customHeight="1" s="48" thickBot="1">
-      <c r="A25" s="12" t="n"/>
-      <c r="B25" s="52" t="n"/>
-      <c r="C25" s="52" t="n"/>
-      <c r="D25" s="52" t="n"/>
-      <c r="E25" s="52" t="n"/>
-      <c r="F25" s="52" t="n"/>
-      <c r="G25" s="52" t="n"/>
-      <c r="H25" s="52" t="n"/>
-      <c r="I25" s="52" t="n"/>
-      <c r="J25" s="9" t="n"/>
-    </row>
-    <row r="26">
-      <c r="J26" s="38" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2309,12 +1805,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="59" t="inlineStr">
+      <c r="A1" s="52" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="59" t="inlineStr">
+      <c r="B1" s="52" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -2367,7 +1863,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>54.93</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -2377,7 +1873,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="8">
@@ -2387,7 +1883,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07155743118038878</v>
+        <v>0.07155486108038436</v>
       </c>
     </row>
     <row r="9">
@@ -2397,7 +1893,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.287409576410747e-05</v>
+        <v>3.291492808074694e-05</v>
       </c>
     </row>
     <row r="10">
@@ -2407,7 +1903,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>74.95704530560798</v>
+        <v>74.95435310300522</v>
       </c>
     </row>
     <row r="11">
@@ -2417,7 +1913,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4497.422718336478</v>
+        <v>4497.261186180313</v>
       </c>
     </row>
     <row r="12">
@@ -2427,7 +1923,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>23229048.98358785</v>
+        <v>23200232.39674906</v>
       </c>
     </row>
     <row r="13">
@@ -2437,7 +1933,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.01110223582802885</v>
+        <v>0.01110237907448234</v>
       </c>
     </row>
     <row r="14">
@@ -2499,7 +1995,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>706.3663630689978</v>
+        <v>706.3247366447951</v>
       </c>
     </row>
     <row r="20">
@@ -2509,7 +2005,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.9680612787663938</v>
+        <v>0.9680389992410972</v>
       </c>
     </row>
     <row r="21">
@@ -2559,7 +2055,43 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9680612787663938</v>
+        <v>0.9680389992410972</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>line_description</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Main Pipe</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>nominal_size</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>material_and_schedule</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2567,7 +2099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2582,22 +2114,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="59" t="inlineStr">
+      <c r="A1" s="52" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="59" t="inlineStr">
+      <c r="B1" s="52" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="C1" s="59" t="inlineStr">
+      <c r="C1" s="52" t="inlineStr">
         <is>
           <t>K/f</t>
         </is>
       </c>
-      <c r="D1" s="59" t="inlineStr">
+      <c r="D1" s="52" t="inlineStr">
         <is>
           <t>nL/D</t>
         </is>

</xml_diff>